<commit_message>
Áramkör tervezés diasorok megosztva.
</commit_message>
<xml_diff>
--- a/pénzes_excel.xlsx
+++ b/pénzes_excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\green\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BME\MSC_SEM_2\RobonAutism\Robonaut\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{57795C6F-CB07-4760-B3D5-35C4B1EC242C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187ACD52-3E74-47C5-BD30-30EA4FB25B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5400" yWindow="240" windowWidth="16200" windowHeight="9308" xr2:uid="{EF0642E4-593F-4BBF-8839-D4AD9E30F0ED}"/>
+    <workbookView xWindow="0" yWindow="1695" windowWidth="21600" windowHeight="11085" xr2:uid="{EF0642E4-593F-4BBF-8839-D4AD9E30F0ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Dávid</t>
   </si>
@@ -51,6 +51,15 @@
   </si>
   <si>
     <t>Lemez</t>
+  </si>
+  <si>
+    <t>AUTos keret</t>
+  </si>
+  <si>
+    <t>Vonalszenzor kártya</t>
+  </si>
+  <si>
+    <t>Motormeghajtó kártya</t>
   </si>
 </sst>
 </file>
@@ -430,18 +439,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7560C3A4-8E38-490B-8570-812DE0470CF7}">
-  <dimension ref="A2:D3"/>
+  <dimension ref="A2:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="18.19921875" customWidth="1"/>
+    <col min="5" max="5" width="12.06640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -454,13 +464,32 @@
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="C3">
         <v>1600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>12000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>